<commit_message>
Changed Cells and Formatting
</commit_message>
<xml_diff>
--- a/simple.xlsx
+++ b/simple.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamkumar/Downloads/xlsx-experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamkumar/Documents/git-repos/xlsx-vcs-experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7F5E764-AEBB-A743-AD7A-6BE506A473BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE13592-9BD7-9F41-83ED-1E89EB3FD3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{F8AF0E36-B0A2-6246-AC5F-329D57F0A160}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45,13 +45,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,20 +416,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09DBE680-9471-814D-8117-32E0BBDAF7A4}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>2</v>
+      <c r="B1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>